<commit_message>
save draft for tmr :D
</commit_message>
<xml_diff>
--- a/Input_table_excel.xlsx
+++ b/Input_table_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sm/Documents/R Training/Healthy_School_Lunch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40967E89-AC71-514A-9A4F-0B5239CB782F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC9201F-BDC0-774E-8CB7-7847F78172FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" xr2:uid="{141BBA30-F381-A340-8159-527D9009D25F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
   <si>
     <t>Group</t>
   </si>
@@ -101,13 +101,7 @@
     <t>Percentage risk that school authority don't support the intervention</t>
   </si>
   <si>
-    <t>Benefit (=)</t>
-  </si>
-  <si>
     <t>Percentage risk that donors don't support the intervention</t>
-  </si>
-  <si>
-    <t>no investment for intervention-&gt; ↑ school authority non-involvement</t>
   </si>
   <si>
     <t>General</t>
@@ -237,6 +231,99 @@
     </r>
   </si>
   <si>
+    <t>Non-compliance of parents due to self-sufficieny (%)</t>
+  </si>
+  <si>
+    <t>Percentage risk that parents provide healthy lunchboxes themselves</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↑risk-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">↓lunch sales </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↑risk-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↓lunch sales</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -&gt; ↓ healthy lunch -&gt; ↓ student eat healthy lunch -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↓ extra benefits from enrollment and external funding</t>
+    </r>
+  </si>
+  <si>
+    <t>Interview with parents</t>
+  </si>
+  <si>
+    <t>Guage interest level, attitude, and behaviour</t>
+  </si>
+  <si>
+    <t>Unskillful workers</t>
+  </si>
+  <si>
+    <t>Non-compliance of students (%)</t>
+  </si>
+  <si>
+    <t>St_noncom</t>
+  </si>
+  <si>
+    <t>Pa_noncom_ng</t>
+  </si>
+  <si>
+    <t>Pa_noncom_sf</t>
+  </si>
+  <si>
+    <t>Percentage risk that students refuse to eat healthy lunch</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↑risk-&gt;  ↓ student eat healthy lunch -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↓ extra benefits from enrollment and external funding</t>
+    </r>
+  </si>
+  <si>
+    <t>Guage attitude, food preference and behaviour of students</t>
+  </si>
+  <si>
+    <t>Interview with teachers and students, literature on eating behaviour based on age (similar study location if any)</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">no lunch_policy (chance_event)-&gt; ↑Parents' noncompliance -&gt; </t>
     </r>
@@ -256,8 +343,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> -&gt; ↓benefit</t>
-    </r>
+      <t xml:space="preserve"> -&gt; ↓benefit; no investment-&gt; cost = cost</t>
+    </r>
+  </si>
+  <si>
+    <t>Benefit (-), Cost (=)</t>
   </si>
   <si>
     <r>
@@ -287,86 +377,47 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>extra benefits from increase enrollment and external funding</t>
-    </r>
-  </si>
-  <si>
-    <t>Interview, past and projected trends (if any) -&gt;Deduction</t>
-  </si>
-  <si>
-    <t>Interveiw, records of similar business model (if any) -&gt; Deduction</t>
-  </si>
-  <si>
-    <t>Pa_nocom_ng</t>
-  </si>
-  <si>
-    <t>Non-compliance of parents due to self-sufficieny (%)</t>
-  </si>
-  <si>
-    <t>Pa_nocom_sf</t>
-  </si>
-  <si>
-    <t>Percentage risk that parents provide healthy lunchboxes themselves</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">↑risk-&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
+      <t xml:space="preserve">extra benefits from increase enrollment and external funding; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t xml:space="preserve">↓lunch sales </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">↑risk-&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>↓lunch sales</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> -&gt; ↓ healthy lunch -&gt; ↓ student eat healthy lunch -&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>↓ extra benefits from enrollment and external funding</t>
-    </r>
-  </si>
-  <si>
-    <t>Interview with parents</t>
-  </si>
-  <si>
-    <t>Guage interest level, attitude, and behaviour</t>
-  </si>
-  <si>
-    <t>Unskillful workers</t>
+      <t>cost = 0</t>
+    </r>
+  </si>
+  <si>
+    <t>Benefit (=), Cost (0)</t>
+  </si>
+  <si>
+    <t>no investment for intervention-&gt; ↑ school authority non-involvement; no investment-&gt; cost = cost</t>
+  </si>
+  <si>
+    <t>Benefit (=), Cost (=)</t>
+  </si>
+  <si>
+    <t>Interveiw with kitchen manager, records of similar business model (if any) -&gt; Deduction</t>
+  </si>
+  <si>
+    <t>Interview with kitchen manager/ cook; past, current, and projected trends (if any) -&gt;Deduction</t>
+  </si>
+  <si>
+    <t>knowledge nutritionist, teacher, kitchen staff</t>
+  </si>
+  <si>
+    <t>Skill kitchen staff</t>
+  </si>
+  <si>
+    <t>corrupted staff?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -390,6 +441,11 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
@@ -737,13 +793,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7035D855-998C-A74D-9C67-1196ED31CC6F}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -755,7 +811,7 @@
     <col min="9" max="9" width="85.1640625" customWidth="1"/>
     <col min="10" max="10" width="121.5" customWidth="1"/>
     <col min="11" max="11" width="22.33203125" customWidth="1"/>
-    <col min="12" max="12" width="57.5" customWidth="1"/>
+    <col min="12" max="12" width="95.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -802,19 +858,19 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
       </c>
       <c r="F2">
         <v>11</v>
@@ -823,88 +879,88 @@
         <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L4" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L5" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -916,7 +972,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -928,21 +984,21 @@
         <v>19</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="K7" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="L7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
@@ -954,21 +1010,21 @@
         <v>20</v>
       </c>
       <c r="J8" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="K8" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="L8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" t="s">
         <v>38</v>
-      </c>
-      <c r="M8" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
@@ -977,108 +1033,149 @@
         <v>17</v>
       </c>
       <c r="I9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J9" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="K9" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="L9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
         <v>41</v>
-      </c>
-      <c r="B11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" t="s">
-        <v>43</v>
       </c>
       <c r="E11" t="s">
         <v>17</v>
       </c>
       <c r="I11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K11" t="s">
         <v>18</v>
       </c>
       <c r="L11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
         <v>17</v>
       </c>
       <c r="I12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="K12" t="s">
         <v>18</v>
       </c>
       <c r="L12" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="M12" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
         <v>17</v>
       </c>
       <c r="I13" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="K13" t="s">
         <v>18</v>
       </c>
       <c r="L13" t="s">
+        <v>59</v>
+      </c>
+      <c r="M13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" t="s">
         <v>67</v>
       </c>
-      <c r="M13" t="s">
+      <c r="K14" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" t="s">
+        <v>69</v>
+      </c>
+      <c r="M14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>69</v>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the risk; in-progress
</commit_message>
<xml_diff>
--- a/Input_table_excel.xlsx
+++ b/Input_table_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sm/Documents/R Training/Healthy_School_Lunch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC9201F-BDC0-774E-8CB7-7847F78172FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB85F43-8E7E-154D-8919-584ED2CA1D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" xr2:uid="{141BBA30-F381-A340-8159-527D9009D25F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="158">
   <si>
     <t>Group</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Project simulation period in years</t>
   </si>
   <si>
-    <t>11 years of primary to highschool graduation in Myanmar</t>
-  </si>
-  <si>
     <t>var_CV</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
   </si>
   <si>
     <t>Guage interest level</t>
-  </si>
-  <si>
-    <t>Ex-post risk</t>
   </si>
   <si>
     <t>Non-compliance</t>
@@ -404,20 +398,617 @@
     <t>Interview with kitchen manager/ cook; past, current, and projected trends (if any) -&gt;Deduction</t>
   </si>
   <si>
-    <t>knowledge nutritionist, teacher, kitchen staff</t>
-  </si>
-  <si>
-    <t>Skill kitchen staff</t>
-  </si>
-  <si>
-    <t>corrupted staff?</t>
+    <t>Extra remark</t>
+  </si>
+  <si>
+    <t>Percentage risk that nurse (nutritionist) does not have enough nutrition knowledge or menu planning skill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assumed to have basic nutrition knowledge as healthcare professional. Head cook to help out in menu planning. If school has no nurse/ nutritionist, this should be included in the base salary. No need extra risk added. </t>
+  </si>
+  <si>
+    <t>Worker_low_skill</t>
+  </si>
+  <si>
+    <t>Percentage risk that kitchen staff will have low nutrition, food safety, hygiene knowledge and inadequate cooking skill</t>
+  </si>
+  <si>
+    <t>Risk low skill (knowledge) of kitchen workers (%)</t>
+  </si>
+  <si>
+    <t>Risk low knowledge of nurse/ nutritionist (%)</t>
+  </si>
+  <si>
+    <t>Cost (+)</t>
+  </si>
+  <si>
+    <t>This is a preventable/ eliminable risk -&gt; consider raising the cost than hurting the benefit</t>
+  </si>
+  <si>
+    <t>not needed (this is a just-in-case scenario. There will be trainings given before service is launched)</t>
+  </si>
+  <si>
+    <t>Kitchen staff can be academic staffs assigned on roster. Consider salary increase for extra responsibility. More base salary if workers are hired. Not advisable to use students as kitchen helpers (This can't be extra curricular)</t>
+  </si>
+  <si>
+    <t>Percentage risk that the head cook (kitchen manager) can't handle the kitchen workflow</t>
+  </si>
+  <si>
+    <t>Percentage risk that food taste bad</t>
+  </si>
+  <si>
+    <t>not needed (this is a just-in-case scenario. There will be menu and taste testing sessions before service is launched)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a preventable/ eliminable risk -&gt; A panel composed of school authority, teachers, parents and students should taste the selected menu prepared by the kitchen team before lunching the service. Only the approved dishes will be included in the menu set. </t>
+  </si>
+  <si>
+    <t>This is a preventable/ eliminable risk -&gt; hire a professional from the start (in small kitchen, head cook/ chef is the kitchen manager as well). Consider replacing instead of training (in case of abrupt resignation -&gt;staff/ assigned teachers will be able to cover short-term if good system is in place.)</t>
+  </si>
+  <si>
+    <t>See N12</t>
+  </si>
+  <si>
+    <t>non-compliance trends can shift through the years-&gt; parents relying more on lunch service or become more self-sufficient, the ranges now may not reflect long-term possibility (new info will come up)-&gt; consider this when choosing the simulation period.</t>
+  </si>
+  <si>
+    <r>
+      <t>Ex-ante risk</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ex-post risk</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Lack of safety</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↑risk-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↑training cost</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↑risk-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↓lunch sales</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (parents concern about food safety), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↓extra benefits from enrollment and external funding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (children don't have/ eat healthy lunch), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↑healthcare costs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (depends if the school has health insurance for students and if the cost of healthcare is borne by the school. But we can still include this considering more students will ask for OTC at nurse's office-&gt; set minimal impact value), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↑food waste and loss</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (discard cooked meals/ discard food due to safety)</t>
+    </r>
+  </si>
+  <si>
+    <t>Benefit (-), Cost (+)</t>
+  </si>
+  <si>
+    <t>This is a preventable/ eliminable risk -&gt; Can operate kitchen only if the safety guidelines are met and there will be routine checks and audits.</t>
+  </si>
+  <si>
+    <t>Set this value low</t>
+  </si>
+  <si>
+    <t>No_safety</t>
+  </si>
+  <si>
+    <t>Percentage risk that food safety and hygiene/ sanitation regulations are not abided by</t>
+  </si>
+  <si>
+    <t>Risk of no food safety, hygiene and sanitation (%)</t>
+  </si>
+  <si>
+    <t>Risk of bad tasting food (%)</t>
+  </si>
+  <si>
+    <t>Risk  low skill (knowledge) of head cook (kitchen manager) (%)</t>
+  </si>
+  <si>
+    <t>Food waste and loss</t>
+  </si>
+  <si>
+    <t>Food_waste_loss</t>
+  </si>
+  <si>
+    <t>Amount of food wasted and lost in USD per year</t>
+  </si>
+  <si>
+    <t>Amount of food waste and loss (USD/yr)</t>
+  </si>
+  <si>
+    <t>This is a base variable</t>
+  </si>
+  <si>
+    <t>No kitchen will have zero food wastage. Hence, this is a base variable.</t>
+  </si>
+  <si>
+    <t>Consider including this in "Loss" group</t>
+  </si>
+  <si>
+    <t>Bad</t>
+  </si>
+  <si>
+    <t>Bad_kitchen_design</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↑risk-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↑training cost</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">↑salary </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(if opt to hire an external professional)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↑risk-&gt;  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↓  lunch sales</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, ↓ student eat healthy lunch -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↓ extra benefits from enrollment and external funding</t>
+    </r>
+  </si>
+  <si>
+    <t>Nu_low_skill</t>
+  </si>
+  <si>
+    <t>Cook_low_skill</t>
+  </si>
+  <si>
+    <t>Food_bad_taste</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↑risk-&gt; potential chance of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">↑salary </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(if opt to hire a better professional who is more expensive)</t>
+    </r>
+  </si>
+  <si>
+    <t>Percentage risk of bad building design</t>
+  </si>
+  <si>
+    <t>Risk of bad kitchen design (%)</t>
+  </si>
+  <si>
+    <t>Risk of bad operation system (%)</t>
+  </si>
+  <si>
+    <t>Risk of bad kitchen installation (%)</t>
+  </si>
+  <si>
+    <t>Risk of bad kitchen equipment (%)</t>
+  </si>
+  <si>
+    <t>Risk of bad kitchen utensils (%)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↑risk-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↑maintenance fee</t>
+    </r>
+  </si>
+  <si>
+    <t>Bad_system</t>
+  </si>
+  <si>
+    <t>Percentage risk of bad operating system</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↑risk-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↑food loss and waste</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↓lunch sales</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (due to ↓productivity and quality)-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">↓extra benefits from enrollment and external funding </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(student not get/ eat healthy lunch)</t>
+    </r>
+  </si>
+  <si>
+    <t>not needed (this is a just-in case scenario. The cost of good building design is included in the installation-&gt; we proceed based on assumption that the design is good)</t>
+  </si>
+  <si>
+    <t>This is a preventable/ eliminable risk -&gt; hire good engineer with good reputation in the first place</t>
+  </si>
+  <si>
+    <t>not needed (this is a just-in-case scenario. We use good money on hiring a competent head cook (kitchen manager)-&gt; inclusive in the base salary)</t>
+  </si>
+  <si>
+    <t>Past literature on food waste and loss; interview with kitchen manager/ cook</t>
+  </si>
+  <si>
+    <t>This is a preventable/ eliminable risk -&gt; hire good manager/ head cook/chef in the first place</t>
+  </si>
+  <si>
+    <t>Bad_installation</t>
+  </si>
+  <si>
+    <t>Percentage risk that eqiupment and systems are improperly installed</t>
+  </si>
+  <si>
+    <t>Bad_equipment</t>
+  </si>
+  <si>
+    <t>Bad_utensil</t>
+  </si>
+  <si>
+    <t>Percentage risk that bad kitchen equipments are bought</t>
+  </si>
+  <si>
+    <t>Percentage risk that bad kitchen utensils are bought</t>
+  </si>
+  <si>
+    <t>not needed (this is a just-in-case scenario. We make sure appropriate items are bought as guided by competent cook and construction manager/ engineer.</t>
+  </si>
+  <si>
+    <t>not needed (this is a just-in-case scenario. We make sure appropriate items are bought as guided by competent cook</t>
+  </si>
+  <si>
+    <t>not needed (this is a just-in-case scenario. We use good money on hiring a competent installation/ construction team.</t>
+  </si>
+  <si>
+    <t>This is a preventable/ eliminable risk.</t>
+  </si>
+  <si>
+    <t>Hazard</t>
+  </si>
+  <si>
+    <t>Risk of natural hazard (%)</t>
+  </si>
+  <si>
+    <t>Risk of power outage (%)</t>
+  </si>
+  <si>
+    <t>Percentage risk of occurance of natural hazard that can result in shutdown of kitchen/ school</t>
+  </si>
+  <si>
+    <t>Percentage risk of power outage (this is included coz cold storage/ freezer is very important)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↑risk-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">↑maintenance fee </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(possible destruction), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↑ food waste and loss</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↓lunch sales</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (short-term)-&gt; the effect may not last long enough to make a signficant dent in nutrition value, so assume no impact on extra enrollment and external funding. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↑risk-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↑food loss and waste</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (most professional kitchens use gas for cooking, so no impact on that) or </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↑fuel usage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (if a generator is used-&gt; preferable but might be too expensive if power outage last extended period of time. An alternative is to buy in small batches-&gt; increase fuel usage as well for more trips make to the market)</t>
+    </r>
+  </si>
+  <si>
+    <t>Interview with residents, check weather history of the specific location</t>
+  </si>
+  <si>
+    <t>This is a location-specific risk. Interveiw with residents or check power supply schedule from local office (if any)</t>
+  </si>
+  <si>
+    <t>Can exclude this risk depending on project location</t>
+  </si>
+  <si>
+    <t>* The values of percentage risks are not the percentage of the risks happening. They are the estimated ranges of the risks' impact on the benefits and costs (i.e. the minimum and maximum vales of the USD gained or lost if the risk occurs, meaning the percent range of risk occurance is considered but not expressed.) The drawback of this is we are assuming the same level of impact for all the variable pairs. This may be overcome by linking the risks straight to cost and benefit (i.e. the impact on each possible variables are considered and estimated before setting the range for each risk).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -448,8 +1039,15 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,6 +1057,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,10 +1085,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,13 +1407,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7035D855-998C-A74D-9C67-1196ED31CC6F}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomRight" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -812,10 +1426,10 @@
     <col min="10" max="10" width="121.5" customWidth="1"/>
     <col min="11" max="11" width="22.33203125" customWidth="1"/>
     <col min="12" max="12" width="95.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.83203125" customWidth="1"/>
+    <col min="13" max="13" width="78.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -855,8 +1469,11 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -864,7 +1481,7 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
@@ -873,10 +1490,10 @@
         <v>25</v>
       </c>
       <c r="F2">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H2">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="I2" t="s">
         <v>26</v>
@@ -891,21 +1508,21 @@
         <v>23</v>
       </c>
       <c r="M2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J3" t="s">
         <v>23</v>
@@ -917,18 +1534,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
         <v>31</v>
-      </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" t="s">
-        <v>32</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -937,21 +1554,21 @@
         <v>23</v>
       </c>
       <c r="L4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
         <v>33</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" t="s">
-        <v>34</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -960,222 +1577,595 @@
         <v>23</v>
       </c>
       <c r="L5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K7" t="s">
-        <v>71</v>
-      </c>
-      <c r="L7" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="I9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
+      <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" t="s">
-        <v>72</v>
-      </c>
-      <c r="K8" t="s">
-        <v>73</v>
-      </c>
-      <c r="L8" t="s">
-        <v>36</v>
-      </c>
-      <c r="M8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" t="s">
-        <v>74</v>
-      </c>
-      <c r="K9" t="s">
-        <v>75</v>
-      </c>
-      <c r="L9" t="s">
-        <v>37</v>
-      </c>
-      <c r="M9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="D11" t="s">
         <v>39</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
       </c>
       <c r="E11" t="s">
         <v>17</v>
       </c>
       <c r="I11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K11" t="s">
         <v>18</v>
       </c>
       <c r="L11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
         <v>17</v>
       </c>
       <c r="I12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K12" t="s">
         <v>18</v>
       </c>
       <c r="L12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="N12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
         <v>17</v>
       </c>
       <c r="I13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K13" t="s">
         <v>18</v>
       </c>
       <c r="L13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>62</v>
-      </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
         <v>17</v>
       </c>
       <c r="I14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K14" t="s">
         <v>18</v>
       </c>
       <c r="L14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
       <c r="D16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D17" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D18" t="s">
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" t="s">
         <v>80</v>
+      </c>
+      <c r="J16" t="s">
+        <v>97</v>
+      </c>
+      <c r="K16" t="s">
+        <v>83</v>
+      </c>
+      <c r="L16" t="s">
+        <v>85</v>
+      </c>
+      <c r="M16" t="s">
+        <v>84</v>
+      </c>
+      <c r="N16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="J19" t="s">
+        <v>98</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" t="s">
+        <v>122</v>
+      </c>
+      <c r="J21" t="s">
+        <v>128</v>
+      </c>
+      <c r="K21" t="s">
+        <v>83</v>
+      </c>
+      <c r="L21" t="s">
+        <v>132</v>
+      </c>
+      <c r="M21" t="s">
+        <v>133</v>
+      </c>
+      <c r="N21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" t="s">
+        <v>130</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K22" t="s">
+        <v>99</v>
+      </c>
+      <c r="L22" t="s">
+        <v>134</v>
+      </c>
+      <c r="M22" t="s">
+        <v>136</v>
+      </c>
+      <c r="N22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" t="s">
+        <v>137</v>
+      </c>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" t="s">
+        <v>138</v>
+      </c>
+      <c r="J23" t="s">
+        <v>128</v>
+      </c>
+      <c r="K23" t="s">
+        <v>83</v>
+      </c>
+      <c r="L23" t="s">
+        <v>145</v>
+      </c>
+      <c r="M23" t="s">
+        <v>146</v>
+      </c>
+      <c r="N23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" t="s">
+        <v>139</v>
+      </c>
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" t="s">
+        <v>141</v>
+      </c>
+      <c r="J24" t="s">
+        <v>128</v>
+      </c>
+      <c r="K24" t="s">
+        <v>83</v>
+      </c>
+      <c r="L24" t="s">
+        <v>143</v>
+      </c>
+      <c r="M24" t="s">
+        <v>146</v>
+      </c>
+      <c r="N24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" t="s">
+        <v>140</v>
+      </c>
+      <c r="E25" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" t="s">
+        <v>142</v>
+      </c>
+      <c r="J25" t="s">
+        <v>128</v>
+      </c>
+      <c r="K25" t="s">
+        <v>83</v>
+      </c>
+      <c r="L25" t="s">
+        <v>144</v>
+      </c>
+      <c r="M25" t="s">
+        <v>146</v>
+      </c>
+      <c r="N25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>147</v>
+      </c>
+      <c r="C26" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" t="s">
+        <v>150</v>
+      </c>
+      <c r="J26" t="s">
+        <v>152</v>
+      </c>
+      <c r="K26" t="s">
+        <v>99</v>
+      </c>
+      <c r="L26" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>149</v>
+      </c>
+      <c r="E27" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" t="s">
+        <v>151</v>
+      </c>
+      <c r="J27" t="s">
+        <v>153</v>
+      </c>
+      <c r="K27" t="s">
+        <v>83</v>
+      </c>
+      <c r="L27" t="s">
+        <v>155</v>
+      </c>
+      <c r="M27" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final first draft-> need to clean up and breakdown
</commit_message>
<xml_diff>
--- a/Input_table_excel.xlsx
+++ b/Input_table_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sm/Documents/R Training/Healthy_School_Lunch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E65335E-8DFC-F446-9307-CC4EB948C818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95D7F5E-4C0E-EA4B-8E13-D8172786E864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" xr2:uid="{141BBA30-F381-A340-8159-527D9009D25F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="346">
   <si>
     <t>Group</t>
   </si>
@@ -1084,9 +1084,6 @@
     </r>
   </si>
   <si>
-    <t>Benefit</t>
-  </si>
-  <si>
     <t>External funding</t>
   </si>
   <si>
@@ -1108,12 +1105,6 @@
     <t>Do_funding</t>
   </si>
   <si>
-    <t xml:space="preserve">Expected funding from individual donors in USD per year </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expected funding from government bodies and organizations in USD per year </t>
-  </si>
-  <si>
     <t>Interview with parents (and teachers)</t>
   </si>
   <si>
@@ -1129,15 +1120,9 @@
     <t>Increased enrollment</t>
   </si>
   <si>
-    <t>Profit from increased enrollment (USD/yr)</t>
-  </si>
-  <si>
     <t>Profit_enrollment</t>
   </si>
   <si>
-    <t>Expected profit from increased enrollment in USD per year</t>
-  </si>
-  <si>
     <t>Interview with parents, teachers and school authority</t>
   </si>
   <si>
@@ -1243,12 +1228,6 @@
     <t>Cost_summer_class</t>
   </si>
   <si>
-    <t>Cost for summer cooking class (%)</t>
-  </si>
-  <si>
-    <t>Percent increased in cost due to summer cooking class (as a fraction of "Cost_training")</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">↑chance-&gt; </t>
     </r>
@@ -1265,21 +1244,12 @@
     <t>Interview with teachers and kitchen manager</t>
   </si>
   <si>
-    <t xml:space="preserve">Estimate extra training costs </t>
-  </si>
-  <si>
     <t>Reduced cost</t>
   </si>
   <si>
-    <t>Saving from reduced cost of supplementary food (USD/yr)</t>
-  </si>
-  <si>
     <t>Saving_supplementary_food</t>
   </si>
   <si>
-    <t>Expected saving from reduced supplmentary food cost in USD per year</t>
-  </si>
-  <si>
     <t>(-) Cost</t>
   </si>
   <si>
@@ -1352,9 +1322,6 @@
     <t>One-time Cost</t>
   </si>
   <si>
-    <t>Recurring Cost</t>
-  </si>
-  <si>
     <t>Utility bills</t>
   </si>
   <si>
@@ -1371,13 +1338,357 @@
   </si>
   <si>
     <t>Supplmentary food will still be provided but cost can be reduced if allocation is based on RDI (e.g. protein will be spread out across the day- if lunch contains more protein, portion of protein food can be reduced for supplementary-&gt; Need to fine-tune based on workout intensity/ schedule)</t>
+  </si>
+  <si>
+    <r>
+      <t>Recurring Cost</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Benefit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Lunch value per unit (USD/unit)</t>
+  </si>
+  <si>
+    <t>Lunch value in USD per unit (*number_student_paid -&gt;Profit_lunchsales; *number_student_unpaid -&gt;Cost (+))</t>
+  </si>
+  <si>
+    <t>(+) Benefit, (+) Cost</t>
+  </si>
+  <si>
+    <t>Cost_electricity</t>
+  </si>
+  <si>
+    <t>Payment for electricity in USD per year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check local rate per unit of electricity </t>
+  </si>
+  <si>
+    <t>Cost_water</t>
+  </si>
+  <si>
+    <t>Payment for water in USD per year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check local rate per unit of water </t>
+  </si>
+  <si>
+    <t>Cost_cooking_gas</t>
+  </si>
+  <si>
+    <t>Payment for cooking gas in USD per year</t>
+  </si>
+  <si>
+    <t>Interview with kitchen manager/ cook and check rate for gas cylinder OR check local rate for gas bill</t>
+  </si>
+  <si>
+    <t>Cost_fuel</t>
+  </si>
+  <si>
+    <t>Cost for summer cooking class (USD/yr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Expected cost for conducting summer cooking class in USD per year</t>
+  </si>
+  <si>
+    <t>Estimate cost for ingredients and materials (ingredients, book/ paper, uniform?, utility bills)</t>
+  </si>
+  <si>
+    <t>Cost of fuel (including fuel use for transport) in USD per year</t>
+  </si>
+  <si>
+    <t>Interview with kitchen manager and school authority</t>
+  </si>
+  <si>
+    <t>For own vehicle, estimate the cost of fuel. For hired vehicle, estimate the cost per trip</t>
+  </si>
+  <si>
+    <t>Ingredients</t>
+  </si>
+  <si>
+    <t>Cost of fresh goods (USD/ yr)</t>
+  </si>
+  <si>
+    <t>Cost_fresh_goods</t>
+  </si>
+  <si>
+    <t>Cost of fresh food (vegetables, fruts, meat, fish, seafood, eggs, milk, etc) in USD per year</t>
+  </si>
+  <si>
+    <t>Cost of dry goods (USD/ yr)</t>
+  </si>
+  <si>
+    <t>Cost_dry_goods</t>
+  </si>
+  <si>
+    <t>Cost of dry goods (rice, lentils, oil, condiments, canned food, etc) in USD per year</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Cost of payment for staff (USD/ yr)</t>
+  </si>
+  <si>
+    <t>Cost_salary</t>
+  </si>
+  <si>
+    <t>Payment for all staff who work in the kitchen in USD per year</t>
+  </si>
+  <si>
+    <t>Monthly salary for new hires; pay increase/ bonus for current hires (academic staff willing take on lunch duty)</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Cost of training (USD/ yr)</t>
+  </si>
+  <si>
+    <t>Cost_training</t>
+  </si>
+  <si>
+    <t>Cost of trainings (cooking, food safety, hygiene and sanitation) for kitchen staff in USD per year</t>
+  </si>
+  <si>
+    <t>Interview with kitchen manager, school nurse/ nutritionist and school authority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food safety trainings should be recurring, anually at least </t>
+  </si>
+  <si>
+    <t>Cost of stationary and other small items (not related to food and beverages) will also be included in training costs. These may include markers, roster board or printed roster sheet, nutrition and hygiene posters for kitchen, etc. Also include petty cash.</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>Cost of maintenance (USD/ yr)</t>
+  </si>
+  <si>
+    <t>Cost_maintenance</t>
+  </si>
+  <si>
+    <t>Cost of kitchen, equipment and system maintenance plus the cost of utensil replacement in USD per year</t>
+  </si>
+  <si>
+    <t>Ask for estimates from kitchen manager and target from school authority</t>
+  </si>
+  <si>
+    <t>Menu printing</t>
+  </si>
+  <si>
+    <t>Cost of menu printing (USD/ yr)</t>
+  </si>
+  <si>
+    <t>Cost_menu_printing</t>
+  </si>
+  <si>
+    <t>Cost of menu printing for parents in USD per year</t>
+  </si>
+  <si>
+    <t>A printed menu with unit price should be given to each parent interested in enrolling their child (included in application package).</t>
+  </si>
+  <si>
+    <t>This cost may be avoided if go digital or ask parents to make decision on the spot during enrollment (but parents may need time to decide)</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>NA (adding base variables)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of students paid for lunch </t>
+  </si>
+  <si>
+    <t>Number_student_paid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of students whose parents pay for lunch service </t>
+  </si>
+  <si>
+    <t>Interview with school authority, parents and teachers</t>
+  </si>
+  <si>
+    <t>Number of students not paid for lunch</t>
+  </si>
+  <si>
+    <t>Number_student_unpaid</t>
+  </si>
+  <si>
+    <t>Number of students whose parents cannot afford but need the lunch service</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↑number-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↑Profit_lunchsales</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↑number-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↓Profit_lunchsales</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>↑cost</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) (deduct from Profit_lunchsales or add to Cost)</t>
+    </r>
+  </si>
+  <si>
+    <t>(-) Benefit or (+) Cost</t>
+  </si>
+  <si>
+    <t>Students whose parents cannot afford lunch service will be cover by the school-&gt; no student will be left out -&gt; Goal is "All Students Get Healthy Lunch"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current funding from government bodies and organizations in USD per year </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current funding from individual donors in USD per year </t>
+  </si>
+  <si>
+    <t>Current profit from increased enrollment in USD per year</t>
+  </si>
+  <si>
+    <t>(+) no intervention</t>
+  </si>
+  <si>
+    <t>Ask for past records from school authority</t>
+  </si>
+  <si>
+    <t>Profit from enrollment (USD/yr)</t>
+  </si>
+  <si>
+    <t>Increased funding from organization (%)</t>
+  </si>
+  <si>
+    <t>Og_increased_funding</t>
+  </si>
+  <si>
+    <t>Increased funding from individual donors (%)</t>
+  </si>
+  <si>
+    <t>Do_increased_funding</t>
+  </si>
+  <si>
+    <t>Increased profit from increased enrollment (%)</t>
+  </si>
+  <si>
+    <t>Profit_increased_enrollment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent increased in funding from government bodies and organizations per year </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent increased in funding from individual donors in USD per year </t>
+  </si>
+  <si>
+    <t>Percent increased in profit from increased enrollment in USD per year</t>
+  </si>
+  <si>
+    <t>Linked to "Do_funding"</t>
+  </si>
+  <si>
+    <t>Linked to "Og_funding"</t>
+  </si>
+  <si>
+    <t>Linked to "Profit_enrollement"</t>
+  </si>
+  <si>
+    <t>Saving from reduced cost of supplementary food (%)</t>
+  </si>
+  <si>
+    <t>Percent saving from reduced supplmentary food cost per year</t>
+  </si>
+  <si>
+    <t>Linked to "Cost_supplementary_food"</t>
+  </si>
+  <si>
+    <t>Cost of supplementary food (USD/ yr)</t>
+  </si>
+  <si>
+    <t>Cost_supplementary_food</t>
+  </si>
+  <si>
+    <t>Current cost of supplementary food in USD per year</t>
+  </si>
+  <si>
+    <t>* Another benefit would be reduced health care costs from better nutrition due to healthy lunch. This benefit would be logical but we don’t know the exact association to quantify the benefit, i.e. because of healthy lunch, we assume students will have more nutrition, will be healthier and less visit to medical centers, leading to reduced cost. But we don't know how long it will take to see the effects of better lunch (since we are not talking about complete dietary change, i.e. we have no control over what the students eat outside school). Nutrition is a long-term process and it can take years or even generations to see the effects. In addition, the effects of nutrition can be overridden by other factors such as infectious diseases (food safety plays a role) and consumption of unhealthy food outside school, etc. Hence, without additional intervention or controls, we cannot make association between healthy lunch and reduced healthcare costs (the association may exist but any quantification of it will be overestimation. May not be advisable. )</t>
+  </si>
+  <si>
+    <t>* Other potential costs would be insurance, tax (if applicable), cost for permits and certification to run the lunch serivce etc. These are not included in this model yet for the sake of simplification.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The estimations will be made based on the current values in Myanmar but the design of the model may not reflect the Myanmar context. This is because the continuation of the lunch service is relied more on the increased funding and donations, and less on income generated from lunch sales- we aim for cheaper and better quality lunch than those offered by outside stalls and price must be maintained (can't increase price since affordibility will be reduced.) </t>
+  </si>
+  <si>
+    <t>(-) no intervention</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1415,8 +1726,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1441,6 +1777,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1454,13 +1796,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1775,22 +2121,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7035D855-998C-A74D-9C67-1196ED31CC6F}">
-  <dimension ref="A1:O124"/>
+  <dimension ref="A1:O74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M41" sqref="M41"/>
+      <selection pane="bottomRight" activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="54" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="50.5" customWidth="1"/>
     <col min="4" max="4" width="24.6640625" customWidth="1"/>
-    <col min="9" max="9" width="85.1640625" customWidth="1"/>
+    <col min="9" max="9" width="91.83203125" customWidth="1"/>
     <col min="10" max="10" width="121.5" customWidth="1"/>
     <col min="11" max="11" width="22.33203125" customWidth="1"/>
     <col min="12" max="12" width="95.1640625" bestFit="1" customWidth="1"/>
@@ -2554,7 +2900,7 @@
         <v>163</v>
       </c>
       <c r="J29" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="K29" t="s">
         <v>165</v>
@@ -2568,16 +2914,16 @@
     </row>
     <row r="30" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C30" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>17</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>164</v>
@@ -2589,7 +2935,7 @@
         <v>57</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
@@ -2603,10 +2949,10 @@
         <v>17</v>
       </c>
       <c r="I31" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="J31" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="K31" t="s">
         <v>169</v>
@@ -2615,24 +2961,24 @@
         <v>170</v>
       </c>
       <c r="M31" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="N31" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C32" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>17</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>171</v>
@@ -2644,401 +2990,844 @@
         <v>170</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D33" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E33" t="s">
         <v>17</v>
       </c>
       <c r="I33" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="J33" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="K33" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="L33" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="M33" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C34" s="4" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>28</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>165</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C35" s="4" t="s">
-        <v>225</v>
+        <v>269</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>226</v>
+        <v>270</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>83</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>229</v>
+        <v>271</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>255</v>
+      </c>
+      <c r="B37" t="s">
         <v>172</v>
       </c>
-      <c r="B37" t="s">
-        <v>173</v>
-      </c>
       <c r="C37" t="s">
-        <v>174</v>
+        <v>324</v>
       </c>
       <c r="D37" t="s">
-        <v>175</v>
+        <v>325</v>
       </c>
       <c r="E37" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="I37" t="s">
+        <v>330</v>
+      </c>
+      <c r="J37" t="s">
+        <v>334</v>
+      </c>
+      <c r="K37" t="s">
+        <v>176</v>
+      </c>
+      <c r="L37" t="s">
+        <v>177</v>
+      </c>
+      <c r="M37" t="s">
+        <v>190</v>
+      </c>
+      <c r="N37" t="s">
         <v>181</v>
-      </c>
-      <c r="J37" t="s">
-        <v>176</v>
-      </c>
-      <c r="K37" t="s">
-        <v>177</v>
-      </c>
-      <c r="L37" t="s">
-        <v>178</v>
-      </c>
-      <c r="M37" t="s">
-        <v>195</v>
-      </c>
-      <c r="N37" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
-        <v>183</v>
+        <v>326</v>
       </c>
       <c r="D38" t="s">
+        <v>327</v>
+      </c>
+      <c r="E38" t="s">
+        <v>17</v>
+      </c>
+      <c r="I38" t="s">
+        <v>331</v>
+      </c>
+      <c r="J38" t="s">
+        <v>333</v>
+      </c>
+      <c r="K38" t="s">
+        <v>176</v>
+      </c>
+      <c r="L38" t="s">
         <v>179</v>
       </c>
-      <c r="E38" t="s">
-        <v>28</v>
-      </c>
-      <c r="I38" t="s">
-        <v>180</v>
-      </c>
-      <c r="J38" t="s">
-        <v>176</v>
-      </c>
-      <c r="K38" t="s">
-        <v>177</v>
-      </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
+        <v>192</v>
+      </c>
+      <c r="N38" t="s">
         <v>182</v>
-      </c>
-      <c r="M38" t="s">
-        <v>197</v>
-      </c>
-      <c r="N38" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
+        <v>183</v>
+      </c>
+      <c r="C39" t="s">
+        <v>328</v>
+      </c>
+      <c r="D39" t="s">
+        <v>329</v>
+      </c>
+      <c r="E39" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" t="s">
+        <v>332</v>
+      </c>
+      <c r="J39" t="s">
+        <v>335</v>
+      </c>
+      <c r="K39" t="s">
+        <v>176</v>
+      </c>
+      <c r="L39" t="s">
+        <v>185</v>
+      </c>
+      <c r="M39" t="s">
         <v>186</v>
       </c>
-      <c r="C39" t="s">
+      <c r="N39" t="s">
         <v>187</v>
       </c>
-      <c r="D39" t="s">
-        <v>188</v>
-      </c>
-      <c r="E39" t="s">
+    </row>
+    <row r="40" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I39" t="s">
-        <v>189</v>
-      </c>
-      <c r="J39" t="s">
+      <c r="I40" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="K40" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="K39" t="s">
-        <v>177</v>
-      </c>
-      <c r="L39" t="s">
-        <v>190</v>
-      </c>
-      <c r="M39" t="s">
-        <v>191</v>
-      </c>
-      <c r="N39" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
-        <v>198</v>
-      </c>
-      <c r="C40" t="s">
-        <v>208</v>
-      </c>
-      <c r="D40" t="s">
-        <v>207</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="L40" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="M40" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I40" t="s">
-        <v>209</v>
-      </c>
-      <c r="J40" t="s">
-        <v>176</v>
-      </c>
-      <c r="K40" t="s">
-        <v>177</v>
-      </c>
-      <c r="L40" t="s">
-        <v>210</v>
-      </c>
-      <c r="M40" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>230</v>
-      </c>
-      <c r="C41" t="s">
-        <v>231</v>
-      </c>
-      <c r="D41" t="s">
-        <v>232</v>
-      </c>
-      <c r="E41" t="s">
-        <v>28</v>
-      </c>
-      <c r="I41" t="s">
+      <c r="I41" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="M41" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>222</v>
+      </c>
+      <c r="C42" t="s">
+        <v>336</v>
+      </c>
+      <c r="D42" t="s">
+        <v>223</v>
+      </c>
+      <c r="E42" t="s">
+        <v>17</v>
+      </c>
+      <c r="I42" t="s">
+        <v>337</v>
+      </c>
+      <c r="J42" t="s">
+        <v>338</v>
+      </c>
+      <c r="K42" t="s">
+        <v>224</v>
+      </c>
+      <c r="L42" t="s">
+        <v>225</v>
+      </c>
+      <c r="M42" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>247</v>
+      </c>
+      <c r="B44" t="s">
+        <v>226</v>
+      </c>
+      <c r="C44" t="s">
         <v>233</v>
       </c>
-      <c r="J41" t="s">
-        <v>176</v>
-      </c>
-      <c r="K41" t="s">
-        <v>234</v>
-      </c>
-      <c r="L41" t="s">
-        <v>235</v>
-      </c>
-      <c r="M41" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>257</v>
-      </c>
-      <c r="B43" t="s">
-        <v>236</v>
-      </c>
-      <c r="C43" t="s">
-        <v>243</v>
-      </c>
-      <c r="D43" t="s">
-        <v>237</v>
-      </c>
-      <c r="E43" t="s">
-        <v>28</v>
-      </c>
-      <c r="I43" t="s">
-        <v>238</v>
-      </c>
-      <c r="J43" t="s">
-        <v>239</v>
-      </c>
-      <c r="K43" t="s">
-        <v>240</v>
-      </c>
-      <c r="L43" t="s">
-        <v>241</v>
-      </c>
-      <c r="M43" t="s">
-        <v>242</v>
-      </c>
-      <c r="N43" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C44" t="s">
-        <v>244</v>
-      </c>
       <c r="D44" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="E44" t="s">
         <v>28</v>
       </c>
       <c r="I44" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="J44" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="K44" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="L44" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="M44" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="N44" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
-        <v>248</v>
-      </c>
       <c r="C45" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="D45" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="E45" t="s">
         <v>28</v>
       </c>
       <c r="I45" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="J45" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="K45" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="L45" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="M45" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="N45" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="C46" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="D46" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="E46" t="s">
         <v>28</v>
       </c>
       <c r="I46" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="J46" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="K46" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="L46" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="M46" t="s">
+        <v>232</v>
+      </c>
+      <c r="N46" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
         <v>242</v>
       </c>
-      <c r="N46" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>258</v>
-      </c>
-      <c r="B48" t="s">
+      <c r="C47" t="s">
+        <v>243</v>
+      </c>
+      <c r="D47" t="s">
+        <v>244</v>
+      </c>
+      <c r="E47" t="s">
+        <v>28</v>
+      </c>
+      <c r="I47" t="s">
+        <v>245</v>
+      </c>
+      <c r="J47" t="s">
+        <v>229</v>
+      </c>
+      <c r="K47" t="s">
+        <v>230</v>
+      </c>
+      <c r="L47" t="s">
+        <v>246</v>
+      </c>
+      <c r="M47" t="s">
+        <v>232</v>
+      </c>
+      <c r="N47" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>254</v>
+      </c>
+      <c r="B49" t="s">
+        <v>248</v>
+      </c>
+      <c r="C49" t="s">
+        <v>249</v>
+      </c>
+      <c r="D49" t="s">
         <v>259</v>
       </c>
-      <c r="C48" t="s">
+      <c r="E49" t="s">
+        <v>28</v>
+      </c>
+      <c r="I49" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C49" t="s">
+      <c r="J49" t="s">
+        <v>111</v>
+      </c>
+      <c r="K49" t="s">
+        <v>230</v>
+      </c>
+      <c r="L49" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
+        <v>250</v>
+      </c>
+      <c r="D50" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="E50" t="s">
+        <v>28</v>
+      </c>
+      <c r="I50" t="s">
+        <v>263</v>
+      </c>
+      <c r="J50" t="s">
+        <v>111</v>
+      </c>
+      <c r="K50" t="s">
+        <v>230</v>
+      </c>
+      <c r="L50" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C51" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A124" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D51" t="s">
+        <v>265</v>
+      </c>
+      <c r="E51" t="s">
+        <v>28</v>
+      </c>
+      <c r="I51" t="s">
+        <v>266</v>
+      </c>
+      <c r="J51" t="s">
+        <v>111</v>
+      </c>
+      <c r="K51" t="s">
+        <v>230</v>
+      </c>
+      <c r="L51" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
+        <v>252</v>
+      </c>
+      <c r="D52" t="s">
+        <v>268</v>
+      </c>
+      <c r="E52" t="s">
+        <v>28</v>
+      </c>
+      <c r="I52" t="s">
+        <v>272</v>
+      </c>
+      <c r="J52" t="s">
+        <v>111</v>
+      </c>
+      <c r="K52" t="s">
+        <v>230</v>
+      </c>
+      <c r="L52" t="s">
+        <v>273</v>
+      </c>
+      <c r="M52" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>275</v>
+      </c>
+      <c r="C53" t="s">
+        <v>276</v>
+      </c>
+      <c r="D53" t="s">
+        <v>277</v>
+      </c>
+      <c r="E53" t="s">
+        <v>28</v>
+      </c>
+      <c r="I53" t="s">
+        <v>278</v>
+      </c>
+      <c r="J53" t="s">
+        <v>111</v>
+      </c>
+      <c r="K53" t="s">
+        <v>230</v>
+      </c>
+      <c r="L53" t="s">
+        <v>273</v>
+      </c>
+      <c r="M53" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>279</v>
+      </c>
+      <c r="D54" t="s">
+        <v>280</v>
+      </c>
+      <c r="E54" t="s">
+        <v>28</v>
+      </c>
+      <c r="I54" t="s">
+        <v>281</v>
+      </c>
+      <c r="J54" t="s">
+        <v>111</v>
+      </c>
+      <c r="K54" t="s">
+        <v>230</v>
+      </c>
+      <c r="L54" t="s">
+        <v>273</v>
+      </c>
+      <c r="M54" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>282</v>
+      </c>
+      <c r="C55" t="s">
+        <v>283</v>
+      </c>
+      <c r="D55" t="s">
+        <v>284</v>
+      </c>
+      <c r="E55" t="s">
+        <v>28</v>
+      </c>
+      <c r="I55" t="s">
+        <v>285</v>
+      </c>
+      <c r="J55" t="s">
+        <v>111</v>
+      </c>
+      <c r="K55" t="s">
+        <v>230</v>
+      </c>
+      <c r="L55" t="s">
+        <v>273</v>
+      </c>
+      <c r="M55" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>287</v>
+      </c>
+      <c r="C56" t="s">
+        <v>288</v>
+      </c>
+      <c r="D56" t="s">
+        <v>289</v>
+      </c>
+      <c r="E56" t="s">
+        <v>28</v>
+      </c>
+      <c r="I56" t="s">
+        <v>290</v>
+      </c>
+      <c r="J56" t="s">
+        <v>111</v>
+      </c>
+      <c r="K56" t="s">
+        <v>230</v>
+      </c>
+      <c r="L56" t="s">
+        <v>291</v>
+      </c>
+      <c r="M56" t="s">
+        <v>292</v>
+      </c>
+      <c r="N56" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>294</v>
+      </c>
+      <c r="C57" t="s">
+        <v>295</v>
+      </c>
+      <c r="D57" t="s">
+        <v>296</v>
+      </c>
+      <c r="E57" t="s">
+        <v>28</v>
+      </c>
+      <c r="I57" t="s">
+        <v>297</v>
+      </c>
+      <c r="J57" t="s">
+        <v>111</v>
+      </c>
+      <c r="K57" t="s">
+        <v>230</v>
+      </c>
+      <c r="L57" t="s">
+        <v>273</v>
+      </c>
+      <c r="M57" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>299</v>
+      </c>
+      <c r="C58" t="s">
+        <v>300</v>
+      </c>
+      <c r="D58" t="s">
+        <v>301</v>
+      </c>
+      <c r="E58" t="s">
+        <v>28</v>
+      </c>
+      <c r="I58" t="s">
+        <v>302</v>
+      </c>
+      <c r="J58" t="s">
+        <v>111</v>
+      </c>
+      <c r="K58" t="s">
+        <v>230</v>
+      </c>
+      <c r="L58" t="s">
+        <v>35</v>
+      </c>
+      <c r="M58" t="s">
+        <v>303</v>
+      </c>
+      <c r="N58" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>305</v>
+      </c>
+      <c r="B60" t="s">
+        <v>306</v>
+      </c>
+      <c r="C60" t="s">
+        <v>307</v>
+      </c>
+      <c r="D60" t="s">
+        <v>308</v>
+      </c>
+      <c r="E60" t="s">
+        <v>28</v>
+      </c>
+      <c r="I60" t="s">
+        <v>309</v>
+      </c>
+      <c r="J60" t="s">
+        <v>314</v>
+      </c>
+      <c r="K60" t="s">
+        <v>176</v>
+      </c>
+      <c r="L60" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C61" t="s">
+        <v>311</v>
+      </c>
+      <c r="D61" t="s">
+        <v>312</v>
+      </c>
+      <c r="E61" t="s">
+        <v>28</v>
+      </c>
+      <c r="I61" t="s">
+        <v>313</v>
+      </c>
+      <c r="J61" t="s">
+        <v>315</v>
+      </c>
+      <c r="K61" t="s">
+        <v>316</v>
+      </c>
+      <c r="L61" t="s">
+        <v>310</v>
+      </c>
+      <c r="M61" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C62" t="s">
+        <v>173</v>
+      </c>
+      <c r="D62" t="s">
+        <v>174</v>
+      </c>
+      <c r="E62" t="s">
+        <v>28</v>
+      </c>
+      <c r="I62" t="s">
+        <v>318</v>
+      </c>
+      <c r="J62" t="s">
+        <v>175</v>
+      </c>
+      <c r="K62" t="s">
+        <v>321</v>
+      </c>
+      <c r="L62" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C63" t="s">
+        <v>180</v>
+      </c>
+      <c r="D63" t="s">
+        <v>178</v>
+      </c>
+      <c r="E63" t="s">
+        <v>28</v>
+      </c>
+      <c r="I63" t="s">
+        <v>319</v>
+      </c>
+      <c r="J63" t="s">
+        <v>175</v>
+      </c>
+      <c r="K63" t="s">
+        <v>321</v>
+      </c>
+      <c r="L63" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C64" t="s">
+        <v>323</v>
+      </c>
+      <c r="D64" t="s">
+        <v>184</v>
+      </c>
+      <c r="E64" t="s">
+        <v>28</v>
+      </c>
+      <c r="I64" t="s">
+        <v>320</v>
+      </c>
+      <c r="J64" t="s">
+        <v>175</v>
+      </c>
+      <c r="K64" t="s">
+        <v>321</v>
+      </c>
+      <c r="L64" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C65" t="s">
+        <v>339</v>
+      </c>
+      <c r="D65" t="s">
+        <v>340</v>
+      </c>
+      <c r="E65" t="s">
+        <v>28</v>
+      </c>
+      <c r="I65" t="s">
+        <v>341</v>
+      </c>
+      <c r="J65" t="s">
+        <v>175</v>
+      </c>
+      <c r="K65" t="s">
+        <v>345</v>
+      </c>
+      <c r="L65" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A70" s="5" t="s">
         <v>157</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A71" s="7" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A72" s="8" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="9" t="s">
+        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change profit_lunchsale to unit_lunch_value
</commit_message>
<xml_diff>
--- a/Input_table_excel.xlsx
+++ b/Input_table_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sm/Documents/R Training/Healthy_School_Lunch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95D7F5E-4C0E-EA4B-8E13-D8172786E864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC53FF1-BD5D-B743-BF12-92A2E888ED11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" xr2:uid="{141BBA30-F381-A340-8159-527D9009D25F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="347">
   <si>
     <t>Group</t>
   </si>
@@ -1682,6 +1682,9 @@
   </si>
   <si>
     <t>(-) no intervention</t>
+  </si>
+  <si>
+    <t>Unit_lunch_value</t>
   </si>
 </sst>
 </file>
@@ -2124,10 +2127,10 @@
   <dimension ref="A1:O74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J67" sqref="J67"/>
+      <selection pane="bottomRight" activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3207,7 +3210,7 @@
         <v>256</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>202</v>
+        <v>346</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>28</v>

</xml_diff>